<commit_message>
withdraw and register camp slots -  refresh not working
Signed-off-by: yajatgulati <yajatgulati01@gmail.com>
</commit_message>
<xml_diff>
--- a/camp_list.xlsx
+++ b/camp_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac8001eaf239fe7a/Documents/NetBeansProjects/CAMs/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -489,16 +489,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="30.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.7265625" style="1"/>
-    <col min="10" max="10" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" style="1" width="8.7265625"/>
+    <col min="2" max="2" customWidth="true" style="1" width="30.54296875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="11.0"/>
+    <col min="4" max="4" customWidth="true" style="1" width="14.7265625"/>
+    <col min="5" max="5" customWidth="true" style="1" width="30.26953125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="21.7265625"/>
+    <col min="7" max="9" style="1" width="8.7265625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="10.26953125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.6328125"/>
+    <col min="12" max="16384" style="1" width="8.7265625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -561,11 +561,11 @@
       <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1">
-        <v>90</v>
-      </c>
-      <c r="I2" s="1">
-        <v>10</v>
+      <c r="H2" s="1" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>9.0</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
@@ -599,11 +599,11 @@
       <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1">
-        <v>90</v>
-      </c>
-      <c r="I3" s="1">
-        <v>10</v>
+      <c r="H3" s="1" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>10.0</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>16</v>
@@ -713,11 +713,11 @@
       <c r="G6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="1">
-        <v>90</v>
-      </c>
-      <c r="I6" s="1">
-        <v>10</v>
+      <c r="H6" s="1" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>10.0</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>29</v>
@@ -751,11 +751,11 @@
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1">
-        <v>10</v>
+      <c r="H7" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>10.0</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>32</v>
@@ -789,11 +789,11 @@
       <c r="G8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1">
-        <v>10</v>
+      <c r="H8" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>10.0</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
allowed camp committee members to generate reports
Signed-off-by: yajatgulati <yajatgulati01@gmail.com>
</commit_message>
<xml_diff>
--- a/camp_list.xlsx
+++ b/camp_list.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -144,6 +144,24 @@
   </si>
   <si>
     <t>NTU</t>
+  </si>
+  <si>
+    <t>OOPs</t>
+  </si>
+  <si>
+    <t>Your MOMS' HOUSE</t>
+  </si>
+  <si>
+    <t>rampant sex</t>
+  </si>
+  <si>
+    <t>OOPsy</t>
+  </si>
+  <si>
+    <t>your mums house</t>
+  </si>
+  <si>
+    <t>lololol</t>
   </si>
 </sst>
 </file>
@@ -188,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -197,6 +215,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -600,7 +620,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>90.0</v>
+        <v>89.0</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>10.0</v>
@@ -803,6 +823,82 @@
       </c>
       <c r="L8" s="1" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B9" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C9" t="n" s="4">
+        <v>45286.0</v>
+      </c>
+      <c r="D9" t="n" s="4">
+        <v>45290.0</v>
+      </c>
+      <c r="E9" t="n" s="4">
+        <v>45285.0</v>
+      </c>
+      <c r="F9" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="H9" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="I9" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="J9" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="K9" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L9" t="b" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B10" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C10" t="n" s="5">
+        <v>45286.0</v>
+      </c>
+      <c r="D10" t="n" s="5">
+        <v>45290.0</v>
+      </c>
+      <c r="E10" t="n" s="5">
+        <v>45285.0</v>
+      </c>
+      <c r="F10" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="H10" t="n" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="I10" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J10" t="s" s="1">
+        <v>41</v>
+      </c>
+      <c r="K10" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L10" t="b" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixed camp commitee member unable to generate report
Signed-off-by: yajatgulati <yajatgulati01@gmail.com>
</commit_message>
<xml_diff>
--- a/camp_list.xlsx
+++ b/camp_list.xlsx
@@ -880,10 +880,10 @@
         <v>40</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>-2.0</v>
+        <v>-3.0</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>41</v>

</xml_diff>